<commit_message>
Cooling and Power supply added to xlsx and README
</commit_message>
<xml_diff>
--- a/Help/tables_for_shop.xlsx
+++ b/Help/tables_for_shop.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\SQL\sql_project\Help\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCA0DDC3-296A-4DA6-BE88-86D635663A73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B58431-F4AA-4F7D-B919-78C124AE3A70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{CFE16DD0-9616-43F0-88C3-6F44FFB5D241}"/>
+    <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{CFE16DD0-9616-43F0-88C3-6F44FFB5D241}"/>
   </bookViews>
   <sheets>
     <sheet name="Processor" sheetId="1" r:id="rId1"/>
     <sheet name="Cooling" sheetId="3" r:id="rId2"/>
-    <sheet name="Graphics card" sheetId="4" r:id="rId3"/>
-    <sheet name="Motherboard" sheetId="2" r:id="rId4"/>
-    <sheet name="RAM" sheetId="5" r:id="rId5"/>
+    <sheet name="Power supply" sheetId="6" r:id="rId3"/>
+    <sheet name="Graphics card" sheetId="4" r:id="rId4"/>
+    <sheet name="Motherboard" sheetId="2" r:id="rId5"/>
+    <sheet name="RAM" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="190">
   <si>
     <t>sku</t>
   </si>
@@ -158,9 +159,6 @@
     <t>GIGABYTE</t>
   </si>
   <si>
-    <t>sockets</t>
-  </si>
-  <si>
     <t>DEEPCOOL</t>
   </si>
   <si>
@@ -531,6 +529,84 @@
   </si>
   <si>
     <t>HyperX FURY RGB</t>
+  </si>
+  <si>
+    <t>Z70</t>
+  </si>
+  <si>
+    <t>DARK ROCK PRO TR4</t>
+  </si>
+  <si>
+    <t>Noctua</t>
+  </si>
+  <si>
+    <t>NH-U9 TR4-SP3</t>
+  </si>
+  <si>
+    <t>output_power</t>
+  </si>
+  <si>
+    <t>FSP</t>
+  </si>
+  <si>
+    <t>PNR PRO 400W</t>
+  </si>
+  <si>
+    <t>DE600 v2</t>
+  </si>
+  <si>
+    <t>Cougar</t>
+  </si>
+  <si>
+    <t>STE 600W</t>
+  </si>
+  <si>
+    <t>Thermaltake</t>
+  </si>
+  <si>
+    <t>Litepower RGB 450W</t>
+  </si>
+  <si>
+    <t>Corsair</t>
+  </si>
+  <si>
+    <t>VS350</t>
+  </si>
+  <si>
+    <t>SYSTEM POWER 9 400W</t>
+  </si>
+  <si>
+    <t>STX750</t>
+  </si>
+  <si>
+    <t>EVGA</t>
+  </si>
+  <si>
+    <t>550 N1</t>
+  </si>
+  <si>
+    <t>Seasonic</t>
+  </si>
+  <si>
+    <t>S12III-650</t>
+  </si>
+  <si>
+    <t>CX550F RGB</t>
+  </si>
+  <si>
+    <t>700 BR</t>
+  </si>
+  <si>
+    <t>Smart PRO RGB 750W</t>
+  </si>
+  <si>
+    <t>TX850M</t>
+  </si>
+  <si>
+    <t>DARK POWER 12 750W</t>
+  </si>
+  <si>
+    <t>DARK POWER 12 1200W</t>
   </si>
 </sst>
 </file>
@@ -1113,10 +1189,10 @@
         <v>10</v>
       </c>
       <c r="D8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" t="s">
         <v>62</v>
-      </c>
-      <c r="E8" t="s">
-        <v>63</v>
       </c>
       <c r="F8">
         <v>10</v>
@@ -1125,7 +1201,7 @@
         <v>16</v>
       </c>
       <c r="H8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I8">
         <v>215</v>
@@ -1145,7 +1221,7 @@
         <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E9" t="s">
         <v>12</v>
@@ -1177,10 +1253,10 @@
         <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F10">
         <v>12</v>
@@ -1241,10 +1317,10 @@
         <v>10</v>
       </c>
       <c r="D12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E12" t="s">
         <v>67</v>
-      </c>
-      <c r="E12" t="s">
-        <v>68</v>
       </c>
       <c r="F12">
         <v>18</v>
@@ -1273,7 +1349,7 @@
         <v>18</v>
       </c>
       <c r="D13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E13" t="s">
         <v>19</v>
@@ -1285,7 +1361,7 @@
         <v>8</v>
       </c>
       <c r="H13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I13">
         <v>35</v>
@@ -1401,10 +1477,10 @@
         <v>18</v>
       </c>
       <c r="D17" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" t="s">
         <v>53</v>
-      </c>
-      <c r="E17" t="s">
-        <v>54</v>
       </c>
       <c r="F17">
         <v>4</v>
@@ -1433,7 +1509,7 @@
         <v>18</v>
       </c>
       <c r="D18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E18" t="s">
         <v>19</v>
@@ -1465,7 +1541,7 @@
         <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E19" t="s">
         <v>19</v>
@@ -1497,10 +1573,10 @@
         <v>18</v>
       </c>
       <c r="D20" t="s">
+        <v>58</v>
+      </c>
+      <c r="E20" t="s">
         <v>59</v>
-      </c>
-      <c r="E20" t="s">
-        <v>60</v>
       </c>
       <c r="F20">
         <v>64</v>
@@ -1529,7 +1605,7 @@
         <v>18</v>
       </c>
       <c r="D21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E21" t="s">
         <v>19</v>
@@ -1560,17 +1636,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A29BB064-0B74-4114-A23E-E9479D7DDEDD}">
-  <dimension ref="B2:H9"/>
+  <dimension ref="B2:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="13.109375" customWidth="1"/>
     <col min="3" max="3" width="17.21875" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="18.5546875" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.3">
@@ -1584,7 +1661,7 @@
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="F2" t="s">
         <v>6</v>
@@ -1601,150 +1678,558 @@
         <v>3000</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="F3">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="G3">
-        <v>599</v>
+        <v>899</v>
       </c>
       <c r="H3">
-        <v>20</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="D4" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F4">
-        <v>150</v>
+        <v>250</v>
       </c>
       <c r="G4">
-        <v>4299</v>
+        <v>5299</v>
       </c>
       <c r="H4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E5" t="s">
         <v>19</v>
       </c>
       <c r="F5">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="G5">
-        <v>799</v>
+        <v>2599</v>
       </c>
       <c r="H5">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D6" t="s">
-        <v>47</v>
+        <v>165</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="F6">
-        <v>130</v>
+        <v>250</v>
       </c>
       <c r="G6">
-        <v>2599</v>
+        <v>7499</v>
       </c>
       <c r="H6">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D7" t="s">
-        <v>49</v>
+        <v>164</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="F7">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="G7">
-        <v>899</v>
+        <v>750</v>
       </c>
       <c r="H7">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D8" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8">
+        <v>110</v>
+      </c>
+      <c r="G8">
+        <v>799</v>
+      </c>
+      <c r="H8">
         <v>12</v>
-      </c>
-      <c r="F8">
-        <v>130</v>
-      </c>
-      <c r="G8">
-        <v>1299</v>
-      </c>
-      <c r="H8">
-        <v>8</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D9" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="E9" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F9">
-        <v>250</v>
+        <v>150</v>
       </c>
       <c r="G9">
-        <v>5299</v>
+        <v>4299</v>
       </c>
       <c r="H9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10">
+        <v>100</v>
+      </c>
+      <c r="G10">
+        <v>599</v>
+      </c>
+      <c r="H10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11">
+        <v>130</v>
+      </c>
+      <c r="G11">
+        <v>1299</v>
+      </c>
+      <c r="H11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>166</v>
+      </c>
+      <c r="D12" t="s">
+        <v>167</v>
+      </c>
+      <c r="E12" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12">
+        <v>180</v>
+      </c>
+      <c r="G12">
+        <v>8999</v>
+      </c>
+      <c r="H12">
         <v>1</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C3:H12">
+    <sortCondition ref="C3:C12"/>
+    <sortCondition ref="E3:E12"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3C5A1D5-3258-4733-8CA6-CAC1CBBBADB4}">
+  <dimension ref="B2:G17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="13.21875" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>168</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>6100</v>
+      </c>
+      <c r="C3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E3">
+        <v>400</v>
+      </c>
+      <c r="F3">
+        <v>3950</v>
+      </c>
+      <c r="G3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>6101</v>
+      </c>
+      <c r="C4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" t="s">
+        <v>188</v>
+      </c>
+      <c r="E4">
+        <v>750</v>
+      </c>
+      <c r="F4">
+        <v>19999</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>6102</v>
+      </c>
+      <c r="C5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" t="s">
+        <v>189</v>
+      </c>
+      <c r="E5">
+        <v>1200</v>
+      </c>
+      <c r="F5">
+        <v>39999</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>6200</v>
+      </c>
+      <c r="C6" t="s">
+        <v>176</v>
+      </c>
+      <c r="D6" t="s">
+        <v>177</v>
+      </c>
+      <c r="E6">
+        <v>350</v>
+      </c>
+      <c r="F6">
+        <v>3699</v>
+      </c>
+      <c r="G6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>6201</v>
+      </c>
+      <c r="C7" t="s">
+        <v>176</v>
+      </c>
+      <c r="D7" t="s">
+        <v>184</v>
+      </c>
+      <c r="E7">
+        <v>550</v>
+      </c>
+      <c r="F7">
+        <v>6049</v>
+      </c>
+      <c r="G7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>6202</v>
+      </c>
+      <c r="C8" t="s">
+        <v>176</v>
+      </c>
+      <c r="D8" t="s">
+        <v>187</v>
+      </c>
+      <c r="E8">
+        <v>850</v>
+      </c>
+      <c r="F8">
+        <v>12999</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>6300</v>
+      </c>
+      <c r="C9" t="s">
+        <v>172</v>
+      </c>
+      <c r="D9" t="s">
+        <v>173</v>
+      </c>
+      <c r="E9">
+        <v>600</v>
+      </c>
+      <c r="F9">
+        <v>2799</v>
+      </c>
+      <c r="G9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>6301</v>
+      </c>
+      <c r="C10" t="s">
+        <v>172</v>
+      </c>
+      <c r="D10" t="s">
+        <v>179</v>
+      </c>
+      <c r="E10">
+        <v>750</v>
+      </c>
+      <c r="F10">
+        <v>4999</v>
+      </c>
+      <c r="G10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>6400</v>
+      </c>
+      <c r="C11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" t="s">
+        <v>171</v>
+      </c>
+      <c r="E11">
+        <v>450</v>
+      </c>
+      <c r="F11">
+        <v>2750</v>
+      </c>
+      <c r="G11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>6500</v>
+      </c>
+      <c r="C12" t="s">
+        <v>180</v>
+      </c>
+      <c r="D12" t="s">
+        <v>181</v>
+      </c>
+      <c r="E12">
+        <v>550</v>
+      </c>
+      <c r="F12">
+        <v>4999</v>
+      </c>
+      <c r="G12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>6501</v>
+      </c>
+      <c r="C13" t="s">
+        <v>180</v>
+      </c>
+      <c r="D13" t="s">
+        <v>185</v>
+      </c>
+      <c r="E13">
+        <v>700</v>
+      </c>
+      <c r="F13">
+        <v>6399</v>
+      </c>
+      <c r="G13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>6600</v>
+      </c>
+      <c r="C14" t="s">
+        <v>169</v>
+      </c>
+      <c r="D14" t="s">
+        <v>170</v>
+      </c>
+      <c r="E14">
+        <v>400</v>
+      </c>
+      <c r="F14">
+        <v>2599</v>
+      </c>
+      <c r="G14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <v>6700</v>
+      </c>
+      <c r="C15" t="s">
+        <v>182</v>
+      </c>
+      <c r="D15" t="s">
+        <v>183</v>
+      </c>
+      <c r="E15">
+        <v>650</v>
+      </c>
+      <c r="F15">
+        <v>5950</v>
+      </c>
+      <c r="G15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>6800</v>
+      </c>
+      <c r="C16" t="s">
+        <v>174</v>
+      </c>
+      <c r="D16" t="s">
+        <v>175</v>
+      </c>
+      <c r="E16">
+        <v>450</v>
+      </c>
+      <c r="F16">
+        <v>3099</v>
+      </c>
+      <c r="G16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <v>6801</v>
+      </c>
+      <c r="C17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D17" t="s">
+        <v>186</v>
+      </c>
+      <c r="E17">
+        <v>750</v>
+      </c>
+      <c r="F17">
+        <v>7899</v>
+      </c>
+      <c r="G17">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C3:G17">
+    <sortCondition ref="C3:C17"/>
+    <sortCondition ref="E3:E17"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C573BB2-15C4-4D3E-9FF1-9D465362C727}">
   <dimension ref="B2:J21"/>
   <sheetViews>
@@ -1765,22 +2250,22 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
         <v>113</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" t="s">
-        <v>114</v>
       </c>
       <c r="G2" t="s">
         <v>30</v>
       </c>
       <c r="H2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I2" t="s">
         <v>7</v>
@@ -1800,13 +2285,13 @@
         <v>39</v>
       </c>
       <c r="E3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F3">
         <v>8</v>
       </c>
       <c r="G3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H3">
         <v>282</v>
@@ -1829,13 +2314,13 @@
         <v>39</v>
       </c>
       <c r="E4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F4">
         <v>6</v>
       </c>
       <c r="G4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H4">
         <v>228</v>
@@ -1858,13 +2343,13 @@
         <v>32</v>
       </c>
       <c r="E5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F5">
         <v>8</v>
       </c>
       <c r="G5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H5">
         <v>238</v>
@@ -1887,13 +2372,13 @@
         <v>32</v>
       </c>
       <c r="E6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F6">
         <v>12</v>
       </c>
       <c r="G6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H6">
         <v>279</v>
@@ -1910,19 +2395,19 @@
         <v>3210</v>
       </c>
       <c r="C7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D7" t="s">
         <v>37</v>
       </c>
       <c r="E7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F7">
         <v>6</v>
       </c>
       <c r="G7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H7">
         <v>174</v>
@@ -1939,19 +2424,19 @@
         <v>3211</v>
       </c>
       <c r="C8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D8" t="s">
         <v>37</v>
       </c>
       <c r="E8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F8">
         <v>6</v>
       </c>
       <c r="G8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H8">
         <v>206</v>
@@ -1968,19 +2453,19 @@
         <v>3220</v>
       </c>
       <c r="C9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D9" t="s">
         <v>39</v>
       </c>
       <c r="E9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F9">
         <v>6</v>
       </c>
       <c r="G9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H9">
         <v>226</v>
@@ -1997,19 +2482,19 @@
         <v>3221</v>
       </c>
       <c r="C10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D10" t="s">
         <v>39</v>
       </c>
       <c r="E10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F10">
         <v>12</v>
       </c>
       <c r="G10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H10">
         <v>319</v>
@@ -2026,19 +2511,19 @@
         <v>3230</v>
       </c>
       <c r="C11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F11">
         <v>4</v>
       </c>
       <c r="G11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H11">
         <v>196</v>
@@ -2055,19 +2540,19 @@
         <v>3240</v>
       </c>
       <c r="C12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D12" t="s">
         <v>32</v>
       </c>
       <c r="E12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F12">
         <v>2</v>
       </c>
       <c r="G12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H12">
         <v>150</v>
@@ -2084,19 +2569,19 @@
         <v>3241</v>
       </c>
       <c r="C13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D13" t="s">
         <v>32</v>
       </c>
       <c r="E13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F13">
         <v>6</v>
       </c>
       <c r="G13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H13">
         <v>247</v>
@@ -2113,19 +2598,19 @@
         <v>3242</v>
       </c>
       <c r="C14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D14" t="s">
         <v>32</v>
       </c>
       <c r="E14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F14">
         <v>8</v>
       </c>
       <c r="G14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H14">
         <v>235</v>
@@ -2142,19 +2627,19 @@
         <v>3243</v>
       </c>
       <c r="C15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D15" t="s">
         <v>32</v>
       </c>
       <c r="E15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F15">
         <v>10</v>
       </c>
       <c r="G15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H15">
         <v>323</v>
@@ -2171,19 +2656,19 @@
         <v>3250</v>
       </c>
       <c r="C16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D16" t="s">
+        <v>130</v>
+      </c>
+      <c r="E16" t="s">
         <v>131</v>
-      </c>
-      <c r="E16" t="s">
-        <v>132</v>
       </c>
       <c r="F16">
         <v>12</v>
       </c>
       <c r="G16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H16">
         <v>245</v>
@@ -2200,19 +2685,19 @@
         <v>3251</v>
       </c>
       <c r="C17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F17">
         <v>8</v>
       </c>
       <c r="G17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H17">
         <v>304</v>
@@ -2229,19 +2714,19 @@
         <v>3252</v>
       </c>
       <c r="C18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E18" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F18">
         <v>8</v>
       </c>
       <c r="G18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H18">
         <v>304</v>
@@ -2258,19 +2743,19 @@
         <v>3253</v>
       </c>
       <c r="C19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F19">
         <v>10</v>
       </c>
       <c r="G19" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H19">
         <v>304</v>
@@ -2287,19 +2772,19 @@
         <v>3254</v>
       </c>
       <c r="C20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D20" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E20" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F20">
         <v>24</v>
       </c>
       <c r="G20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H20">
         <v>304</v>
@@ -2316,19 +2801,19 @@
         <v>3260</v>
       </c>
       <c r="C21" t="s">
+        <v>115</v>
+      </c>
+      <c r="D21" t="s">
         <v>116</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
+        <v>120</v>
+      </c>
+      <c r="F21">
+        <v>2</v>
+      </c>
+      <c r="G21" t="s">
         <v>117</v>
-      </c>
-      <c r="E21" t="s">
-        <v>121</v>
-      </c>
-      <c r="F21">
-        <v>2</v>
-      </c>
-      <c r="G21" t="s">
-        <v>118</v>
       </c>
       <c r="H21">
         <v>146</v>
@@ -2349,7 +2834,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E3392A4-9E6F-42E3-97B8-A18420C6FB12}">
   <dimension ref="B2:L23"/>
   <sheetViews>
@@ -2389,7 +2874,7 @@
         <v>30</v>
       </c>
       <c r="H2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I2" t="s">
         <v>31</v>
@@ -2409,16 +2894,16 @@
         <v>2400</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E3" t="s">
         <v>25</v>
       </c>
       <c r="F3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G3" t="s">
         <v>34</v>
@@ -2444,19 +2929,19 @@
         <v>2401</v>
       </c>
       <c r="C4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" t="s">
         <v>70</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" t="s">
         <v>71</v>
       </c>
-      <c r="E4" t="s">
-        <v>54</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>72</v>
-      </c>
-      <c r="G4" t="s">
-        <v>73</v>
       </c>
       <c r="H4">
         <v>2</v>
@@ -2479,16 +2964,16 @@
         <v>2402</v>
       </c>
       <c r="C5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E5" t="s">
         <v>19</v>
       </c>
       <c r="F5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G5" t="s">
         <v>34</v>
@@ -2497,7 +2982,7 @@
         <v>4</v>
       </c>
       <c r="I5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J5">
         <v>2</v>
@@ -2514,16 +2999,16 @@
         <v>2403</v>
       </c>
       <c r="C6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E6" t="s">
         <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G6" t="s">
         <v>34</v>
@@ -2532,7 +3017,7 @@
         <v>4</v>
       </c>
       <c r="I6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J6">
         <v>2</v>
@@ -2549,16 +3034,16 @@
         <v>2404</v>
       </c>
       <c r="C7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E7" t="s">
         <v>19</v>
       </c>
       <c r="F7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G7" t="s">
         <v>34</v>
@@ -2567,7 +3052,7 @@
         <v>4</v>
       </c>
       <c r="I7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J7">
         <v>3</v>
@@ -2587,13 +3072,13 @@
         <v>37</v>
       </c>
       <c r="D8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E8" t="s">
         <v>12</v>
       </c>
       <c r="F8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G8" t="s">
         <v>34</v>
@@ -2622,7 +3107,7 @@
         <v>37</v>
       </c>
       <c r="D9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E9" t="s">
         <v>12</v>
@@ -2657,13 +3142,13 @@
         <v>37</v>
       </c>
       <c r="D10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E10" t="s">
         <v>12</v>
       </c>
       <c r="F10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G10" t="s">
         <v>34</v>
@@ -2672,7 +3157,7 @@
         <v>4</v>
       </c>
       <c r="I10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J10">
         <v>4</v>
@@ -2692,13 +3177,13 @@
         <v>37</v>
       </c>
       <c r="D11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E11" t="s">
         <v>25</v>
       </c>
       <c r="F11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G11" t="s">
         <v>34</v>
@@ -2707,7 +3192,7 @@
         <v>4</v>
       </c>
       <c r="I11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J11">
         <v>2</v>
@@ -2727,13 +3212,13 @@
         <v>37</v>
       </c>
       <c r="D12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E12" t="s">
         <v>19</v>
       </c>
       <c r="F12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G12" t="s">
         <v>34</v>
@@ -2742,7 +3227,7 @@
         <v>4</v>
       </c>
       <c r="I12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J12">
         <v>1</v>
@@ -2762,13 +3247,13 @@
         <v>37</v>
       </c>
       <c r="D13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E13" t="s">
         <v>22</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G13" t="s">
         <v>34</v>
@@ -2777,7 +3262,7 @@
         <v>8</v>
       </c>
       <c r="I13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J13">
         <v>1</v>
@@ -2797,13 +3282,13 @@
         <v>39</v>
       </c>
       <c r="D14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E14" t="s">
         <v>12</v>
       </c>
       <c r="F14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G14" t="s">
         <v>34</v>
@@ -2812,7 +3297,7 @@
         <v>4</v>
       </c>
       <c r="I14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J14">
         <v>2</v>
@@ -2832,13 +3317,13 @@
         <v>39</v>
       </c>
       <c r="D15" t="s">
+        <v>87</v>
+      </c>
+      <c r="E15" t="s">
+        <v>67</v>
+      </c>
+      <c r="F15" t="s">
         <v>88</v>
-      </c>
-      <c r="E15" t="s">
-        <v>68</v>
-      </c>
-      <c r="F15" t="s">
-        <v>89</v>
       </c>
       <c r="G15" t="s">
         <v>34</v>
@@ -2847,7 +3332,7 @@
         <v>8</v>
       </c>
       <c r="I15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J15">
         <v>2</v>
@@ -2867,22 +3352,22 @@
         <v>39</v>
       </c>
       <c r="D16" t="s">
+        <v>90</v>
+      </c>
+      <c r="E16" t="s">
+        <v>62</v>
+      </c>
+      <c r="F16" t="s">
         <v>91</v>
       </c>
-      <c r="E16" t="s">
-        <v>63</v>
-      </c>
-      <c r="F16" t="s">
-        <v>92</v>
-      </c>
       <c r="G16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H16">
         <v>4</v>
       </c>
       <c r="I16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J16">
         <v>3</v>
@@ -2902,22 +3387,22 @@
         <v>39</v>
       </c>
       <c r="D17" t="s">
+        <v>92</v>
+      </c>
+      <c r="E17" t="s">
+        <v>62</v>
+      </c>
+      <c r="F17" t="s">
+        <v>91</v>
+      </c>
+      <c r="G17" t="s">
         <v>93</v>
-      </c>
-      <c r="E17" t="s">
-        <v>63</v>
-      </c>
-      <c r="F17" t="s">
-        <v>92</v>
-      </c>
-      <c r="G17" t="s">
-        <v>94</v>
       </c>
       <c r="H17">
         <v>4</v>
       </c>
       <c r="I17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J17">
         <v>5</v>
@@ -2937,13 +3422,13 @@
         <v>39</v>
       </c>
       <c r="D18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E18" t="s">
         <v>19</v>
       </c>
       <c r="F18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G18" t="s">
         <v>34</v>
@@ -2952,7 +3437,7 @@
         <v>2</v>
       </c>
       <c r="I18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J18">
         <v>1</v>
@@ -2972,13 +3457,13 @@
         <v>39</v>
       </c>
       <c r="D19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E19" t="s">
         <v>19</v>
       </c>
       <c r="F19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G19" t="s">
         <v>34</v>
@@ -2987,7 +3472,7 @@
         <v>2</v>
       </c>
       <c r="I19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J19">
         <v>3</v>
@@ -3007,13 +3492,13 @@
         <v>39</v>
       </c>
       <c r="D20" t="s">
+        <v>109</v>
+      </c>
+      <c r="E20" t="s">
+        <v>59</v>
+      </c>
+      <c r="F20" t="s">
         <v>110</v>
-      </c>
-      <c r="E20" t="s">
-        <v>60</v>
-      </c>
-      <c r="F20" t="s">
-        <v>111</v>
       </c>
       <c r="G20" t="s">
         <v>34</v>
@@ -3022,7 +3507,7 @@
         <v>8</v>
       </c>
       <c r="I20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J20">
         <v>4</v>
@@ -3042,7 +3527,7 @@
         <v>32</v>
       </c>
       <c r="D21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E21" t="s">
         <v>12</v>
@@ -3077,7 +3562,7 @@
         <v>32</v>
       </c>
       <c r="D22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E22" t="s">
         <v>12</v>
@@ -3112,13 +3597,13 @@
         <v>32</v>
       </c>
       <c r="D23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E23" t="s">
         <v>19</v>
       </c>
       <c r="F23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G23" t="s">
         <v>34</v>
@@ -3149,7 +3634,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F29FFB0B-451A-4C6F-A283-7DD392B2BC87}">
   <dimension ref="B2:J27"/>
   <sheetViews>
@@ -3181,13 +3666,13 @@
         <v>30</v>
       </c>
       <c r="F2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I2" t="s">
         <v>7</v>
@@ -3201,7 +3686,7 @@
         <v>4100</v>
       </c>
       <c r="C3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E3" t="s">
         <v>34</v>
@@ -3227,7 +3712,7 @@
         <v>4101</v>
       </c>
       <c r="C4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E4" t="s">
         <v>34</v>
@@ -3253,10 +3738,10 @@
         <v>4200</v>
       </c>
       <c r="C5" t="s">
+        <v>159</v>
+      </c>
+      <c r="D5" t="s">
         <v>160</v>
-      </c>
-      <c r="D5" t="s">
-        <v>161</v>
       </c>
       <c r="E5" t="s">
         <v>34</v>
@@ -3282,10 +3767,10 @@
         <v>4201</v>
       </c>
       <c r="C6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E6" t="s">
         <v>34</v>
@@ -3311,7 +3796,7 @@
         <v>4300</v>
       </c>
       <c r="C7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E7" t="s">
         <v>34</v>
@@ -3337,7 +3822,7 @@
         <v>4301</v>
       </c>
       <c r="C8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E8" t="s">
         <v>34</v>
@@ -3363,13 +3848,13 @@
         <v>4400</v>
       </c>
       <c r="C9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F9">
         <v>2</v>
@@ -3392,13 +3877,13 @@
         <v>4401</v>
       </c>
       <c r="C10" t="s">
+        <v>145</v>
+      </c>
+      <c r="D10" t="s">
         <v>146</v>
       </c>
-      <c r="D10" t="s">
-        <v>147</v>
-      </c>
       <c r="E10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F10">
         <v>4</v>
@@ -3421,13 +3906,13 @@
         <v>4402</v>
       </c>
       <c r="C11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F11">
         <v>8</v>
@@ -3450,10 +3935,10 @@
         <v>4403</v>
       </c>
       <c r="C12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E12" t="s">
         <v>34</v>
@@ -3479,10 +3964,10 @@
         <v>4404</v>
       </c>
       <c r="C13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E13" t="s">
         <v>34</v>
@@ -3508,10 +3993,10 @@
         <v>4405</v>
       </c>
       <c r="C14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E14" t="s">
         <v>34</v>
@@ -3537,10 +4022,10 @@
         <v>4406</v>
       </c>
       <c r="C15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E15" t="s">
         <v>34</v>
@@ -3566,10 +4051,10 @@
         <v>4407</v>
       </c>
       <c r="C16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E16" t="s">
         <v>34</v>
@@ -3595,10 +4080,10 @@
         <v>4408</v>
       </c>
       <c r="C17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D17" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E17" t="s">
         <v>34</v>
@@ -3624,10 +4109,10 @@
         <v>4409</v>
       </c>
       <c r="C18" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D18" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E18" t="s">
         <v>34</v>
@@ -3653,10 +4138,10 @@
         <v>4410</v>
       </c>
       <c r="C19" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E19" t="s">
         <v>34</v>
@@ -3682,10 +4167,10 @@
         <v>4411</v>
       </c>
       <c r="C20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D20" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E20" t="s">
         <v>34</v>
@@ -3711,10 +4196,10 @@
         <v>4500</v>
       </c>
       <c r="C21" t="s">
+        <v>154</v>
+      </c>
+      <c r="D21" t="s">
         <v>155</v>
-      </c>
-      <c r="D21" t="s">
-        <v>156</v>
       </c>
       <c r="E21" t="s">
         <v>34</v>
@@ -3740,10 +4225,10 @@
         <v>4501</v>
       </c>
       <c r="C22" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D22" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E22" t="s">
         <v>34</v>
@@ -3769,10 +4254,10 @@
         <v>4502</v>
       </c>
       <c r="C23" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D23" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E23" t="s">
         <v>34</v>
@@ -3798,10 +4283,10 @@
         <v>4503</v>
       </c>
       <c r="C24" t="s">
+        <v>154</v>
+      </c>
+      <c r="D24" t="s">
         <v>155</v>
-      </c>
-      <c r="D24" t="s">
-        <v>156</v>
       </c>
       <c r="E24" t="s">
         <v>34</v>
@@ -3827,10 +4312,10 @@
         <v>4504</v>
       </c>
       <c r="C25" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E25" t="s">
         <v>34</v>
@@ -3856,7 +4341,7 @@
         <v>4601</v>
       </c>
       <c r="C26" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E26" t="s">
         <v>34</v>
@@ -3882,7 +4367,7 @@
         <v>4602</v>
       </c>
       <c r="C27" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E27" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
Added to Readme, xslx and drawio are ended
</commit_message>
<xml_diff>
--- a/Help/tables_for_shop.xlsx
+++ b/Help/tables_for_shop.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\SQL\sql_project\Help\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B58431-F4AA-4F7D-B919-78C124AE3A70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16319C63-89E2-45BE-A739-442B20E7B7C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{CFE16DD0-9616-43F0-88C3-6F44FFB5D241}"/>
+    <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" activeTab="8" xr2:uid="{CFE16DD0-9616-43F0-88C3-6F44FFB5D241}"/>
   </bookViews>
   <sheets>
     <sheet name="Processor" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,9 @@
     <sheet name="Graphics card" sheetId="4" r:id="rId4"/>
     <sheet name="Motherboard" sheetId="2" r:id="rId5"/>
     <sheet name="RAM" sheetId="5" r:id="rId6"/>
+    <sheet name="SSD" sheetId="7" r:id="rId7"/>
+    <sheet name="HDD" sheetId="8" r:id="rId8"/>
+    <sheet name="Case" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="227">
   <si>
     <t>sku</t>
   </si>
@@ -607,6 +610,117 @@
   </si>
   <si>
     <t>DARK POWER 12 1200W</t>
+  </si>
+  <si>
+    <t>capacity</t>
+  </si>
+  <si>
+    <t>A400</t>
+  </si>
+  <si>
+    <t>m.2</t>
+  </si>
+  <si>
+    <t>KC2500</t>
+  </si>
+  <si>
+    <t>860 EVO</t>
+  </si>
+  <si>
+    <t>"2.5"</t>
+  </si>
+  <si>
+    <t>870 EVO</t>
+  </si>
+  <si>
+    <t>KC600</t>
+  </si>
+  <si>
+    <t>870 QVO</t>
+  </si>
+  <si>
+    <t>rotations_speed</t>
+  </si>
+  <si>
+    <t>WD</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>"3.5"</t>
+  </si>
+  <si>
+    <t>Seagate</t>
+  </si>
+  <si>
+    <t>BarraCuda</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>Blue Mobile</t>
+  </si>
+  <si>
+    <t>BarraCuda Pro</t>
+  </si>
+  <si>
+    <t>Red Plus</t>
+  </si>
+  <si>
+    <t>SkyHawk</t>
+  </si>
+  <si>
+    <t>graphic_card_length</t>
+  </si>
+  <si>
+    <t>Aerocool</t>
+  </si>
+  <si>
+    <t>Bolt Mini</t>
+  </si>
+  <si>
+    <t>MG120-G</t>
+  </si>
+  <si>
+    <t>Glider-G</t>
+  </si>
+  <si>
+    <t>Standatr-ATX</t>
+  </si>
+  <si>
+    <t>MasterBox K501L</t>
+  </si>
+  <si>
+    <t>E_SHIELD</t>
+  </si>
+  <si>
+    <t>QBX</t>
+  </si>
+  <si>
+    <t>Versa T35 TG RGB</t>
+  </si>
+  <si>
+    <t>Carbide Series SPEC-DELTA RGB</t>
+  </si>
+  <si>
+    <t>Fractal Design</t>
+  </si>
+  <si>
+    <t>Core 2300</t>
+  </si>
+  <si>
+    <t>MATREXX 55 MESH ADD-RGB 4F</t>
+  </si>
+  <si>
+    <t>NZXT</t>
+  </si>
+  <si>
+    <t>PURE BASE 500 Window</t>
+  </si>
+  <si>
+    <t>The Tower 100</t>
   </si>
 </sst>
 </file>
@@ -657,9 +771,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1639,7 +1755,7 @@
   <dimension ref="B2:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1889,8 +2005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3C5A1D5-3258-4733-8CA6-CAC1CBBBADB4}">
   <dimension ref="B2:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2839,7 +2955,7 @@
   <dimension ref="B2:L23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3639,7 +3755,7 @@
   <dimension ref="B2:J27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4395,4 +4511,905 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{470FD739-B7EA-4AE3-ABAD-620811A00A00}">
+  <dimension ref="B2:K11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>7110</v>
+      </c>
+      <c r="C3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D3" t="s">
+        <v>191</v>
+      </c>
+      <c r="E3">
+        <v>480</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="G3">
+        <v>3699</v>
+      </c>
+      <c r="H3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>7111</v>
+      </c>
+      <c r="C4" t="s">
+        <v>145</v>
+      </c>
+      <c r="D4" t="s">
+        <v>197</v>
+      </c>
+      <c r="E4">
+        <v>1024</v>
+      </c>
+      <c r="F4" t="s">
+        <v>195</v>
+      </c>
+      <c r="G4">
+        <v>11499</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>7120</v>
+      </c>
+      <c r="C5" t="s">
+        <v>145</v>
+      </c>
+      <c r="D5" t="s">
+        <v>191</v>
+      </c>
+      <c r="E5">
+        <v>240</v>
+      </c>
+      <c r="F5" t="s">
+        <v>192</v>
+      </c>
+      <c r="G5">
+        <v>1799</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>7121</v>
+      </c>
+      <c r="C6" t="s">
+        <v>145</v>
+      </c>
+      <c r="D6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E6">
+        <v>250</v>
+      </c>
+      <c r="F6" t="s">
+        <v>192</v>
+      </c>
+      <c r="G6">
+        <v>3499</v>
+      </c>
+      <c r="H6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>7122</v>
+      </c>
+      <c r="C7" t="s">
+        <v>145</v>
+      </c>
+      <c r="D7" t="s">
+        <v>193</v>
+      </c>
+      <c r="E7">
+        <v>1000</v>
+      </c>
+      <c r="F7" t="s">
+        <v>192</v>
+      </c>
+      <c r="G7">
+        <v>9899</v>
+      </c>
+      <c r="H7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>7210</v>
+      </c>
+      <c r="C8" t="s">
+        <v>150</v>
+      </c>
+      <c r="D8" t="s">
+        <v>196</v>
+      </c>
+      <c r="E8">
+        <v>250</v>
+      </c>
+      <c r="F8" t="s">
+        <v>195</v>
+      </c>
+      <c r="G8">
+        <v>5099</v>
+      </c>
+      <c r="H8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>7211</v>
+      </c>
+      <c r="C9" t="s">
+        <v>150</v>
+      </c>
+      <c r="D9" t="s">
+        <v>198</v>
+      </c>
+      <c r="E9">
+        <v>4000</v>
+      </c>
+      <c r="F9" t="s">
+        <v>195</v>
+      </c>
+      <c r="G9">
+        <v>36499</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="K9" s="2"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>7220</v>
+      </c>
+      <c r="C10" t="s">
+        <v>150</v>
+      </c>
+      <c r="D10" t="s">
+        <v>194</v>
+      </c>
+      <c r="E10">
+        <v>250</v>
+      </c>
+      <c r="F10" t="s">
+        <v>192</v>
+      </c>
+      <c r="G10">
+        <v>4199</v>
+      </c>
+      <c r="H10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>7221</v>
+      </c>
+      <c r="C11" t="s">
+        <v>150</v>
+      </c>
+      <c r="D11">
+        <v>980</v>
+      </c>
+      <c r="E11">
+        <v>500</v>
+      </c>
+      <c r="F11" t="s">
+        <v>192</v>
+      </c>
+      <c r="G11">
+        <v>6199</v>
+      </c>
+      <c r="H11">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C3:H11">
+    <sortCondition ref="C3:C11"/>
+    <sortCondition ref="F3:F11"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCC727F5-FE66-447A-90C3-B12CC1C75E40}">
+  <dimension ref="B2:I12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F2" t="s">
+        <v>199</v>
+      </c>
+      <c r="G2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>8100</v>
+      </c>
+      <c r="C3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D3" t="s">
+        <v>204</v>
+      </c>
+      <c r="E3">
+        <v>1000</v>
+      </c>
+      <c r="F3">
+        <v>7200</v>
+      </c>
+      <c r="G3" t="s">
+        <v>202</v>
+      </c>
+      <c r="H3">
+        <v>3299</v>
+      </c>
+      <c r="I3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>8101</v>
+      </c>
+      <c r="C4" t="s">
+        <v>203</v>
+      </c>
+      <c r="D4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E4">
+        <v>500</v>
+      </c>
+      <c r="F4">
+        <v>7200</v>
+      </c>
+      <c r="G4" t="s">
+        <v>195</v>
+      </c>
+      <c r="H4">
+        <v>3199</v>
+      </c>
+      <c r="I4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>8102</v>
+      </c>
+      <c r="C5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D5" t="s">
+        <v>204</v>
+      </c>
+      <c r="E5">
+        <v>2000</v>
+      </c>
+      <c r="F5">
+        <v>5400</v>
+      </c>
+      <c r="G5" t="s">
+        <v>195</v>
+      </c>
+      <c r="H5">
+        <v>5999</v>
+      </c>
+      <c r="I5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>8103</v>
+      </c>
+      <c r="C6" t="s">
+        <v>203</v>
+      </c>
+      <c r="D6" t="s">
+        <v>209</v>
+      </c>
+      <c r="E6">
+        <v>3000</v>
+      </c>
+      <c r="F6">
+        <v>5400</v>
+      </c>
+      <c r="G6" t="s">
+        <v>202</v>
+      </c>
+      <c r="H6">
+        <v>7299</v>
+      </c>
+      <c r="I6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>8200</v>
+      </c>
+      <c r="C7" t="s">
+        <v>200</v>
+      </c>
+      <c r="D7" t="s">
+        <v>201</v>
+      </c>
+      <c r="E7">
+        <v>500</v>
+      </c>
+      <c r="F7">
+        <v>5400</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="H7">
+        <v>2599</v>
+      </c>
+      <c r="I7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>8201</v>
+      </c>
+      <c r="C8" t="s">
+        <v>200</v>
+      </c>
+      <c r="D8" t="s">
+        <v>201</v>
+      </c>
+      <c r="E8">
+        <v>500</v>
+      </c>
+      <c r="F8">
+        <v>7200</v>
+      </c>
+      <c r="G8" t="s">
+        <v>202</v>
+      </c>
+      <c r="H8">
+        <v>2699</v>
+      </c>
+      <c r="I8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>8202</v>
+      </c>
+      <c r="C9" t="s">
+        <v>200</v>
+      </c>
+      <c r="D9" t="s">
+        <v>201</v>
+      </c>
+      <c r="E9">
+        <v>1000</v>
+      </c>
+      <c r="F9">
+        <v>5400</v>
+      </c>
+      <c r="G9" t="s">
+        <v>202</v>
+      </c>
+      <c r="H9">
+        <v>3099</v>
+      </c>
+      <c r="I9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>8203</v>
+      </c>
+      <c r="C10" t="s">
+        <v>200</v>
+      </c>
+      <c r="D10" t="s">
+        <v>205</v>
+      </c>
+      <c r="E10">
+        <v>1000</v>
+      </c>
+      <c r="F10">
+        <v>7200</v>
+      </c>
+      <c r="G10" t="s">
+        <v>202</v>
+      </c>
+      <c r="H10">
+        <v>5499</v>
+      </c>
+      <c r="I10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>8204</v>
+      </c>
+      <c r="C11" t="s">
+        <v>200</v>
+      </c>
+      <c r="D11" t="s">
+        <v>206</v>
+      </c>
+      <c r="E11">
+        <v>500</v>
+      </c>
+      <c r="F11">
+        <v>5400</v>
+      </c>
+      <c r="G11" t="s">
+        <v>195</v>
+      </c>
+      <c r="H11">
+        <v>2950</v>
+      </c>
+      <c r="I11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>8205</v>
+      </c>
+      <c r="C12" t="s">
+        <v>200</v>
+      </c>
+      <c r="D12" t="s">
+        <v>208</v>
+      </c>
+      <c r="E12">
+        <v>3000</v>
+      </c>
+      <c r="F12">
+        <v>5400</v>
+      </c>
+      <c r="G12" t="s">
+        <v>202</v>
+      </c>
+      <c r="H12">
+        <v>6499</v>
+      </c>
+      <c r="I12">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C3:I12">
+    <sortCondition ref="C3:C12"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFAA7708-9BBB-44B3-803C-F39ACEA68726}">
+  <dimension ref="B2:H15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="14.21875" customWidth="1"/>
+    <col min="4" max="4" width="27.6640625" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" customWidth="1"/>
+    <col min="6" max="6" width="18.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" t="s">
+        <v>210</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>9100</v>
+      </c>
+      <c r="C3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D3" t="s">
+        <v>212</v>
+      </c>
+      <c r="E3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3">
+        <v>318</v>
+      </c>
+      <c r="G3">
+        <v>2899</v>
+      </c>
+      <c r="H3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>9101</v>
+      </c>
+      <c r="C4" t="s">
+        <v>211</v>
+      </c>
+      <c r="D4" t="s">
+        <v>214</v>
+      </c>
+      <c r="E4" t="s">
+        <v>215</v>
+      </c>
+      <c r="F4">
+        <v>325</v>
+      </c>
+      <c r="G4">
+        <v>3099</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>9200</v>
+      </c>
+      <c r="C5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" t="s">
+        <v>225</v>
+      </c>
+      <c r="E5" t="s">
+        <v>215</v>
+      </c>
+      <c r="F5">
+        <v>369</v>
+      </c>
+      <c r="G5">
+        <v>7899</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>9300</v>
+      </c>
+      <c r="C6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" t="s">
+        <v>216</v>
+      </c>
+      <c r="E6" t="s">
+        <v>215</v>
+      </c>
+      <c r="F6">
+        <v>410</v>
+      </c>
+      <c r="G6">
+        <v>3599</v>
+      </c>
+      <c r="H6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>9400</v>
+      </c>
+      <c r="C7" t="s">
+        <v>176</v>
+      </c>
+      <c r="D7" t="s">
+        <v>220</v>
+      </c>
+      <c r="E7" t="s">
+        <v>215</v>
+      </c>
+      <c r="F7">
+        <v>330</v>
+      </c>
+      <c r="G7">
+        <v>4999</v>
+      </c>
+      <c r="H7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>9500</v>
+      </c>
+      <c r="C8" t="s">
+        <v>172</v>
+      </c>
+      <c r="D8" t="s">
+        <v>213</v>
+      </c>
+      <c r="E8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8">
+        <v>330</v>
+      </c>
+      <c r="G8">
+        <v>2999</v>
+      </c>
+      <c r="H8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>9501</v>
+      </c>
+      <c r="C9" t="s">
+        <v>172</v>
+      </c>
+      <c r="D9" t="s">
+        <v>218</v>
+      </c>
+      <c r="E9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F9">
+        <v>350</v>
+      </c>
+      <c r="G9">
+        <v>4450</v>
+      </c>
+      <c r="H9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>9600</v>
+      </c>
+      <c r="C10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" t="s">
+        <v>217</v>
+      </c>
+      <c r="E10" t="s">
+        <v>89</v>
+      </c>
+      <c r="F10">
+        <v>370</v>
+      </c>
+      <c r="G10">
+        <v>3750</v>
+      </c>
+      <c r="H10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>9601</v>
+      </c>
+      <c r="C11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" t="s">
+        <v>223</v>
+      </c>
+      <c r="E11" t="s">
+        <v>215</v>
+      </c>
+      <c r="F11">
+        <v>370</v>
+      </c>
+      <c r="G11">
+        <v>5950</v>
+      </c>
+      <c r="H11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>9700</v>
+      </c>
+      <c r="C12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D12" t="s">
+        <v>222</v>
+      </c>
+      <c r="E12" t="s">
+        <v>215</v>
+      </c>
+      <c r="F12">
+        <v>380</v>
+      </c>
+      <c r="G12">
+        <v>5199</v>
+      </c>
+      <c r="H12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>9800</v>
+      </c>
+      <c r="C13" t="s">
+        <v>224</v>
+      </c>
+      <c r="D13" t="s">
+        <v>75</v>
+      </c>
+      <c r="E13" t="s">
+        <v>215</v>
+      </c>
+      <c r="F13">
+        <v>381</v>
+      </c>
+      <c r="G13">
+        <v>6499</v>
+      </c>
+      <c r="H13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>9900</v>
+      </c>
+      <c r="C14" t="s">
+        <v>174</v>
+      </c>
+      <c r="D14" t="s">
+        <v>219</v>
+      </c>
+      <c r="E14" t="s">
+        <v>215</v>
+      </c>
+      <c r="F14">
+        <v>300</v>
+      </c>
+      <c r="G14">
+        <v>4699</v>
+      </c>
+      <c r="H14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <v>9901</v>
+      </c>
+      <c r="C15" t="s">
+        <v>174</v>
+      </c>
+      <c r="D15" t="s">
+        <v>226</v>
+      </c>
+      <c r="E15" t="s">
+        <v>101</v>
+      </c>
+      <c r="F15">
+        <v>330</v>
+      </c>
+      <c r="G15">
+        <v>8799</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C3:H15">
+    <sortCondition ref="C3:C15"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added sku for cooling
</commit_message>
<xml_diff>
--- a/Help/tables_for_shop.xlsx
+++ b/Help/tables_for_shop.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\SQL\sql_project\Help\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16319C63-89E2-45BE-A739-442B20E7B7C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EEDF569-D76B-4644-90CF-D5144C8D6144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" activeTab="8" xr2:uid="{CFE16DD0-9616-43F0-88C3-6F44FFB5D241}"/>
+    <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{CFE16DD0-9616-43F0-88C3-6F44FFB5D241}"/>
   </bookViews>
   <sheets>
     <sheet name="Processor" sheetId="1" r:id="rId1"/>
@@ -1754,8 +1754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A29BB064-0B74-4114-A23E-E9479D7DDEDD}">
   <dimension ref="B2:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1791,7 +1791,7 @@
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3">
-        <v>3000</v>
+        <v>5100</v>
       </c>
       <c r="C3" t="s">
         <v>47</v>
@@ -1813,6 +1813,9 @@
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>5200</v>
+      </c>
       <c r="C4" t="s">
         <v>50</v>
       </c>
@@ -1833,6 +1836,9 @@
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>5300</v>
+      </c>
       <c r="C5" t="s">
         <v>45</v>
       </c>
@@ -1853,6 +1859,9 @@
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>5301</v>
+      </c>
       <c r="C6" t="s">
         <v>45</v>
       </c>
@@ -1873,6 +1882,9 @@
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>5400</v>
+      </c>
       <c r="C7" t="s">
         <v>42</v>
       </c>
@@ -1893,6 +1905,9 @@
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>5401</v>
+      </c>
       <c r="C8" t="s">
         <v>42</v>
       </c>
@@ -1913,6 +1928,9 @@
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>5402</v>
+      </c>
       <c r="C9" t="s">
         <v>42</v>
       </c>
@@ -1933,6 +1951,9 @@
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>5500</v>
+      </c>
       <c r="C10" t="s">
         <v>40</v>
       </c>
@@ -1953,6 +1974,9 @@
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>5501</v>
+      </c>
       <c r="C11" t="s">
         <v>40</v>
       </c>
@@ -1973,6 +1997,9 @@
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>5600</v>
+      </c>
       <c r="C12" t="s">
         <v>166</v>
       </c>
@@ -3755,7 +3782,7 @@
   <dimension ref="B2:J27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5072,7 +5099,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFAA7708-9BBB-44B3-803C-F39ACEA68726}">
   <dimension ref="B2:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added check of compatibility of components. Fixed wrong data in case_pc
</commit_message>
<xml_diff>
--- a/Help/tables_for_shop.xlsx
+++ b/Help/tables_for_shop.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\SQL\sql_project\Help\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EEDF569-D76B-4644-90CF-D5144C8D6144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{877C10F4-E541-49B5-8FA1-5CEAE5223707}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{CFE16DD0-9616-43F0-88C3-6F44FFB5D241}"/>
+    <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" activeTab="8" xr2:uid="{CFE16DD0-9616-43F0-88C3-6F44FFB5D241}"/>
   </bookViews>
   <sheets>
     <sheet name="Processor" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="226">
   <si>
     <t>sku</t>
   </si>
@@ -685,9 +685,6 @@
   </si>
   <si>
     <t>Glider-G</t>
-  </si>
-  <si>
-    <t>Standatr-ATX</t>
   </si>
   <si>
     <t>MasterBox K501L</t>
@@ -1754,7 +1751,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A29BB064-0B74-4114-A23E-E9479D7DDEDD}">
   <dimension ref="B2:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -5099,8 +5096,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFAA7708-9BBB-44B3-803C-F39ACEA68726}">
   <dimension ref="B2:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5168,7 +5165,7 @@
         <v>214</v>
       </c>
       <c r="E4" t="s">
-        <v>215</v>
+        <v>79</v>
       </c>
       <c r="F4">
         <v>325</v>
@@ -5188,10 +5185,10 @@
         <v>45</v>
       </c>
       <c r="D5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E5" t="s">
-        <v>215</v>
+        <v>79</v>
       </c>
       <c r="F5">
         <v>369</v>
@@ -5211,10 +5208,10 @@
         <v>42</v>
       </c>
       <c r="D6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E6" t="s">
-        <v>215</v>
+        <v>79</v>
       </c>
       <c r="F6">
         <v>410</v>
@@ -5234,10 +5231,10 @@
         <v>176</v>
       </c>
       <c r="D7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E7" t="s">
-        <v>215</v>
+        <v>79</v>
       </c>
       <c r="F7">
         <v>330</v>
@@ -5280,7 +5277,7 @@
         <v>172</v>
       </c>
       <c r="D9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E9" t="s">
         <v>101</v>
@@ -5303,7 +5300,7 @@
         <v>40</v>
       </c>
       <c r="D10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E10" t="s">
         <v>89</v>
@@ -5326,10 +5323,10 @@
         <v>40</v>
       </c>
       <c r="D11" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E11" t="s">
-        <v>215</v>
+        <v>79</v>
       </c>
       <c r="F11">
         <v>370</v>
@@ -5346,13 +5343,13 @@
         <v>9700</v>
       </c>
       <c r="C12" t="s">
+        <v>220</v>
+      </c>
+      <c r="D12" t="s">
         <v>221</v>
       </c>
-      <c r="D12" t="s">
-        <v>222</v>
-      </c>
       <c r="E12" t="s">
-        <v>215</v>
+        <v>79</v>
       </c>
       <c r="F12">
         <v>380</v>
@@ -5369,13 +5366,13 @@
         <v>9800</v>
       </c>
       <c r="C13" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D13" t="s">
         <v>75</v>
       </c>
       <c r="E13" t="s">
-        <v>215</v>
+        <v>79</v>
       </c>
       <c r="F13">
         <v>381</v>
@@ -5395,10 +5392,10 @@
         <v>174</v>
       </c>
       <c r="D14" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E14" t="s">
-        <v>215</v>
+        <v>79</v>
       </c>
       <c r="F14">
         <v>300</v>
@@ -5418,7 +5415,7 @@
         <v>174</v>
       </c>
       <c r="D15" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E15" t="s">
         <v>101</v>

</xml_diff>